<commit_message>
removed 100% gpa from the file
</commit_message>
<xml_diff>
--- a/Student Performance Survey - March 2025.xlsx
+++ b/Student Performance Survey - March 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emrulhasan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manan\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248AB6F3-C740-1345-AF56-817D3180106D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CBDD02-E319-4D3F-8E9A-140F5BA7AAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="16860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -1925,13 +1925,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AB176" sqref="AB176"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="71.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.109375" customWidth="1"/>
+    <col min="4" max="4" width="87" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="101.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="92.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="119.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="105.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="106.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="111.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="88.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="88.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="127.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="132.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="108.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2044,7 +2063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
@@ -2157,7 +2176,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
@@ -2270,7 +2289,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>79</v>
       </c>
@@ -2383,7 +2402,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>87</v>
       </c>
@@ -2496,7 +2515,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:37" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>95</v>
       </c>
@@ -2609,7 +2628,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>108</v>
       </c>
@@ -2722,7 +2741,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
@@ -2835,7 +2854,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>118</v>
       </c>
@@ -2948,7 +2967,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>125</v>
       </c>
@@ -3061,7 +3080,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>128</v>
       </c>
@@ -3174,7 +3193,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>133</v>
       </c>
@@ -3287,7 +3306,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>140</v>
       </c>
@@ -3400,7 +3419,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>147</v>
       </c>
@@ -3513,7 +3532,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>155</v>
       </c>
@@ -3626,7 +3645,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>159</v>
       </c>
@@ -3739,7 +3758,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>162</v>
       </c>
@@ -3852,7 +3871,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:37" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>165</v>
       </c>
@@ -3965,7 +3984,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>171</v>
       </c>
@@ -4078,7 +4097,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>175</v>
       </c>
@@ -4191,7 +4210,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>175</v>
       </c>
@@ -4304,7 +4323,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>183</v>
       </c>
@@ -4417,7 +4436,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>187</v>
       </c>
@@ -4530,7 +4549,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>189</v>
       </c>
@@ -4643,7 +4662,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>191</v>
       </c>
@@ -4756,7 +4775,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>194</v>
       </c>
@@ -4869,7 +4888,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>201</v>
       </c>
@@ -4982,7 +5001,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>202</v>
       </c>
@@ -5095,7 +5114,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>206</v>
       </c>
@@ -5208,7 +5227,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>208</v>
       </c>
@@ -5321,7 +5340,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>210</v>
       </c>
@@ -5434,7 +5453,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>212</v>
       </c>
@@ -5547,7 +5566,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>140</v>
       </c>
@@ -5660,7 +5679,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>218</v>
       </c>
@@ -5773,7 +5792,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>221</v>
       </c>
@@ -5886,7 +5905,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>223</v>
       </c>
@@ -5999,7 +6018,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>226</v>
       </c>
@@ -6112,7 +6131,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:37" ht="48" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>228</v>
       </c>
@@ -6225,7 +6244,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>191</v>
       </c>
@@ -6338,7 +6357,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>234</v>
       </c>
@@ -6451,7 +6470,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>64</v>
       </c>
@@ -6564,7 +6583,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>240</v>
       </c>
@@ -6677,7 +6696,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="43" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>210</v>
       </c>
@@ -6790,7 +6809,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>245</v>
       </c>
@@ -6903,7 +6922,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>123</v>
       </c>
@@ -7016,7 +7035,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>189</v>
       </c>
@@ -7129,7 +7148,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>257</v>
       </c>
@@ -7242,7 +7261,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>258</v>
       </c>
@@ -7355,7 +7374,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>132</v>
       </c>
@@ -7468,7 +7487,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>262</v>
       </c>
@@ -7581,7 +7600,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>271</v>
       </c>
@@ -7694,7 +7713,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>206</v>
       </c>
@@ -7807,7 +7826,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>128</v>
       </c>
@@ -7920,7 +7939,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>128</v>
       </c>
@@ -8033,7 +8052,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>276</v>
       </c>
@@ -8146,7 +8165,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>278</v>
       </c>
@@ -8259,7 +8278,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:37" ht="48" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>128</v>
       </c>
@@ -8372,7 +8391,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>284</v>
       </c>
@@ -8485,7 +8504,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>286</v>
       </c>
@@ -8598,7 +8617,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>288</v>
       </c>
@@ -8711,7 +8730,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>291</v>
       </c>
@@ -8824,7 +8843,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>297</v>
       </c>
@@ -8937,7 +8956,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>301</v>
       </c>
@@ -9050,7 +9069,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>205</v>
       </c>
@@ -9163,7 +9182,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>308</v>
       </c>
@@ -9276,7 +9295,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="66" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>262</v>
       </c>
@@ -9389,7 +9408,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="67" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>311</v>
       </c>
@@ -9502,7 +9521,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>87</v>
       </c>
@@ -9615,7 +9634,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>87</v>
       </c>
@@ -9728,7 +9747,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="1:37" ht="176" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:37" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>315</v>
       </c>
@@ -9841,7 +9860,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>323</v>
       </c>
@@ -9954,7 +9973,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>189</v>
       </c>
@@ -10067,7 +10086,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>87</v>
       </c>
@@ -10180,7 +10199,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="74" spans="1:37" ht="112" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:37" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>329</v>
       </c>
@@ -10293,7 +10312,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>332</v>
       </c>
@@ -10406,7 +10425,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="76" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>335</v>
       </c>
@@ -10519,7 +10538,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="77" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>343</v>
       </c>
@@ -10632,7 +10651,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="78" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>346</v>
       </c>
@@ -10745,7 +10764,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>128</v>
       </c>
@@ -10858,7 +10877,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="80" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>349</v>
       </c>
@@ -10971,7 +10990,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="81" spans="1:37" ht="48" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>360</v>
       </c>
@@ -11084,7 +11103,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="82" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>87</v>
       </c>
@@ -11197,7 +11216,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>194</v>
       </c>
@@ -11310,7 +11329,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>194</v>
       </c>
@@ -11423,7 +11442,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>189</v>
       </c>
@@ -11536,7 +11555,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="86" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>240</v>
       </c>
@@ -11649,7 +11668,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="87" spans="1:37" ht="208" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:37" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>368</v>
       </c>
@@ -11762,7 +11781,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="88" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>370</v>
       </c>
@@ -11875,7 +11894,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="89" spans="1:37" ht="48" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>371</v>
       </c>
@@ -11988,7 +12007,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="90" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>87</v>
       </c>
@@ -12101,7 +12120,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="91" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>373</v>
       </c>
@@ -12214,7 +12233,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="1:37" ht="112" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:37" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>374</v>
       </c>
@@ -12327,7 +12346,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="93" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>205</v>
       </c>
@@ -12440,7 +12459,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="94" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>44</v>
       </c>
@@ -12553,7 +12572,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="95" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:37" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>54</v>
       </c>
@@ -12666,7 +12685,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>329</v>
       </c>
@@ -12779,7 +12798,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="97" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>383</v>
       </c>
@@ -12892,7 +12911,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="98" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>183</v>
       </c>
@@ -13005,7 +13024,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="99" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>123</v>
       </c>
@@ -13118,7 +13137,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="100" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>123</v>
       </c>
@@ -13231,7 +13250,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="101" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>389</v>
       </c>
@@ -13344,7 +13363,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="102" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>393</v>
       </c>
@@ -13457,7 +13476,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="103" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>183</v>
       </c>
@@ -13570,7 +13589,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="104" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:37" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>395</v>
       </c>
@@ -13683,7 +13702,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="105" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>175</v>
       </c>
@@ -13796,7 +13815,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="106" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>128</v>
       </c>
@@ -13909,7 +13928,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="107" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>406</v>
       </c>
@@ -14022,7 +14041,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="108" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>374</v>
       </c>
@@ -14135,7 +14154,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="109" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>414</v>
       </c>
@@ -14248,7 +14267,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="110" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>234</v>
       </c>
@@ -14361,7 +14380,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="111" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>159</v>
       </c>
@@ -14474,7 +14493,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="112" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>346</v>
       </c>
@@ -14587,7 +14606,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="113" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>416</v>
       </c>
@@ -14700,7 +14719,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>284</v>
       </c>
@@ -14813,7 +14832,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="115" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>228</v>
       </c>
@@ -14926,7 +14945,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="116" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>162</v>
       </c>
@@ -15039,7 +15058,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="117" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>205</v>
       </c>
@@ -15152,7 +15171,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>194</v>
       </c>
@@ -15265,7 +15284,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="119" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>406</v>
       </c>
@@ -15378,7 +15397,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="120" spans="1:37" ht="48" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>422</v>
       </c>
@@ -15491,7 +15510,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="121" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>424</v>
       </c>
@@ -15604,7 +15623,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="122" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>426</v>
       </c>
@@ -15717,7 +15736,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="123" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>406</v>
       </c>
@@ -15830,7 +15849,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="124" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>128</v>
       </c>
@@ -15943,7 +15962,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="125" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>435</v>
       </c>
@@ -16056,7 +16075,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="126" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>437</v>
       </c>
@@ -16169,7 +16188,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="127" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>308</v>
       </c>
@@ -16282,7 +16301,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="128" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>443</v>
       </c>
@@ -16395,7 +16414,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="129" spans="1:37" ht="48" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>202</v>
       </c>
@@ -16508,7 +16527,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="130" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>240</v>
       </c>
@@ -16621,7 +16640,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="131" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>346</v>
       </c>
@@ -16734,7 +16753,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="132" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>370</v>
       </c>
@@ -16847,7 +16866,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="133" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>448</v>
       </c>
@@ -16960,7 +16979,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="134" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>426</v>
       </c>
@@ -17073,7 +17092,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="135" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>453</v>
       </c>
@@ -17186,7 +17205,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="136" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>128</v>
       </c>
@@ -17299,7 +17318,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="137" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>123</v>
       </c>
@@ -17412,7 +17431,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>183</v>
       </c>
@@ -17525,7 +17544,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="139" spans="1:37" ht="48" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>329</v>
       </c>
@@ -17638,7 +17657,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="140" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>374</v>
       </c>
@@ -17751,7 +17770,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="141" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>140</v>
       </c>
@@ -17864,7 +17883,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="142" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>123</v>
       </c>
@@ -17977,7 +17996,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="143" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>183</v>
       </c>
@@ -18090,7 +18109,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="144" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>459</v>
       </c>
@@ -18203,7 +18222,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="145" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>218</v>
       </c>
@@ -18316,7 +18335,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="146" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>463</v>
       </c>
@@ -18429,7 +18448,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="147" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>123</v>
       </c>
@@ -18542,7 +18561,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="148" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>79</v>
       </c>
@@ -18655,7 +18674,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="149" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>469</v>
       </c>
@@ -18768,7 +18787,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="150" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>277</v>
       </c>
@@ -18881,7 +18900,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="151" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>371</v>
       </c>
@@ -18994,7 +19013,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="152" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>473</v>
       </c>
@@ -19107,7 +19126,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="153" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>183</v>
       </c>
@@ -19220,7 +19239,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="154" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>474</v>
       </c>
@@ -19333,7 +19352,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="155" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>38</v>
       </c>
@@ -19446,7 +19465,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="156" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>191</v>
       </c>
@@ -19559,7 +19578,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="157" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>477</v>
       </c>
@@ -19672,7 +19691,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="158" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>380</v>
       </c>
@@ -19785,7 +19804,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="159" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>206</v>
       </c>
@@ -19898,7 +19917,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="160" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>205</v>
       </c>
@@ -20011,7 +20030,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="161" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>87</v>
       </c>
@@ -20124,7 +20143,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="162" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>189</v>
       </c>
@@ -20237,7 +20256,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="163" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>481</v>
       </c>
@@ -20350,7 +20369,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="164" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>483</v>
       </c>
@@ -20463,7 +20482,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="165" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>123</v>
       </c>
@@ -20576,7 +20595,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="166" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>245</v>
       </c>
@@ -20689,7 +20708,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="167" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>87</v>
       </c>
@@ -20802,7 +20821,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="168" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>485</v>
       </c>
@@ -20915,7 +20934,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="169" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>487</v>
       </c>
@@ -21028,7 +21047,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="170" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>489</v>
       </c>
@@ -21141,7 +21160,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="171" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>257</v>
       </c>
@@ -21254,7 +21273,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="172" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>183</v>
       </c>
@@ -21367,7 +21386,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="173" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>206</v>
       </c>
@@ -21480,7 +21499,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="174" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>84</v>
       </c>
@@ -21593,7 +21612,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="175" spans="1:37" ht="112" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:37" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>284</v>
       </c>
@@ -21706,7 +21725,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="176" spans="1:37" ht="80" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:37" ht="72" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>498</v>
       </c>
@@ -21819,7 +21838,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="177" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>500</v>
       </c>
@@ -21932,7 +21951,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="178" spans="1:37" ht="144" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:37" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>502</v>
       </c>
@@ -22045,7 +22064,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="179" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>48</v>
       </c>
@@ -22158,7 +22177,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="180" spans="1:37" ht="64" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:37" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>483</v>
       </c>

</xml_diff>